<commit_message>
Material Update | Wildlife Ecology
Added 90 new questions.
</commit_message>
<xml_diff>
--- a/PrePTEL/PrePTEL/Materials/Wildlife Ecology.xlsx
+++ b/PrePTEL/PrePTEL/Materials/Wildlife Ecology.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamaf\Desktop\空白\プロジェクツ\NPTEL Quiz\Materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamaf\Desktop\空白\プロジェクツ\PrePTEL\Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A3A53B-1D35-4DD9-BD1E-609EB60AC2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7600C3D7-9F91-446D-8367-8CA72161B336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="445">
   <si>
     <t>Which of these is not a characteristic of fitness?</t>
   </si>
@@ -265,6 +265,1101 @@
   </si>
   <si>
     <t>experiments</t>
+  </si>
+  <si>
+    <t>Tick Hunting</t>
+  </si>
+  <si>
+    <t>Auto Grooming</t>
+  </si>
+  <si>
+    <t>Allo Grooming</t>
+  </si>
+  <si>
+    <t>Foraging</t>
+  </si>
+  <si>
+    <t>Behaviorism</t>
+  </si>
+  <si>
+    <t>Ecology</t>
+  </si>
+  <si>
+    <t>Ethology</t>
+  </si>
+  <si>
+    <t>Prey-Predator Dynamics</t>
+  </si>
+  <si>
+    <t>Mutualism</t>
+  </si>
+  <si>
+    <t>Amensalism</t>
+  </si>
+  <si>
+    <t>Commensalism</t>
+  </si>
+  <si>
+    <t>Protocooperation</t>
+  </si>
+  <si>
+    <t>Colony</t>
+  </si>
+  <si>
+    <t>Allelopathy</t>
+  </si>
+  <si>
+    <t>rB &lt; C</t>
+  </si>
+  <si>
+    <t>rB &gt; C</t>
+  </si>
+  <si>
+    <t>rB = C</t>
+  </si>
+  <si>
+    <t>rB + C = 0</t>
+  </si>
+  <si>
+    <t>Infraspecific Competition</t>
+  </si>
+  <si>
+    <t>Apparent Competition</t>
+  </si>
+  <si>
+    <t>Disguised Competition</t>
+  </si>
+  <si>
+    <t>Harmonious Competition</t>
+  </si>
+  <si>
+    <t>Ecogram</t>
+  </si>
+  <si>
+    <t>Ethogram</t>
+  </si>
+  <si>
+    <t>Behaviourogram</t>
+  </si>
+  <si>
+    <t>Animalogram</t>
+  </si>
+  <si>
+    <t>I observe a bird take a tick out of another bird's head and eat it. In the social context, this behavior is known as __________.</t>
+  </si>
+  <si>
+    <t>The scientific study of animal behavior is known as __________.</t>
+  </si>
+  <si>
+    <t>Trampling of grass due to movement of animals is an example of __________.</t>
+  </si>
+  <si>
+    <t>Birds on a giraffe is an example of __________.</t>
+  </si>
+  <si>
+    <t>I observe a monkey take a tick out of another monkey's head and eat it. In the social context, this behavior would be called __________.</t>
+  </si>
+  <si>
+    <t>Hamilton's rule can be stated as __________.</t>
+  </si>
+  <si>
+    <t>Egrets with buffaloes are an example of __________.</t>
+  </si>
+  <si>
+    <t>The interaction between exotic shrubs and trees through the action of seed predators is an example of __________.</t>
+  </si>
+  <si>
+    <t>Harmonious interaction occurs where __________.</t>
+  </si>
+  <si>
+    <t>at least one participant is benefited</t>
+  </si>
+  <si>
+    <t>at least one participant is unharmed</t>
+  </si>
+  <si>
+    <t>both participants are benefited</t>
+  </si>
+  <si>
+    <t>both participants are unharmed</t>
+  </si>
+  <si>
+    <t>An inventory of behaviors exhibited by an animal during a behavior exercise is called __________.</t>
+  </si>
+  <si>
+    <t>Upright Pyramid of Numbers</t>
+  </si>
+  <si>
+    <t>Inverted Pyramid of Numbers</t>
+  </si>
+  <si>
+    <t>Spindle Pyramid of Numbers</t>
+  </si>
+  <si>
+    <t>Dumbbell Pyramid of Numbers</t>
+  </si>
+  <si>
+    <t>10% Rule</t>
+  </si>
+  <si>
+    <t>1% Rule</t>
+  </si>
+  <si>
+    <t>Trophic Cascade</t>
+  </si>
+  <si>
+    <t>Biodiversity</t>
+  </si>
+  <si>
+    <t>Eutrophic Lakes</t>
+  </si>
+  <si>
+    <t>Hypereutrophic Lakes</t>
+  </si>
+  <si>
+    <t>Oligotrophic Lakes</t>
+  </si>
+  <si>
+    <t>Mesotrophic Lakes</t>
+  </si>
+  <si>
+    <t>Frog Is a Consumer and Carnivore</t>
+  </si>
+  <si>
+    <t>Frog Is a Consumer and Herbivore</t>
+  </si>
+  <si>
+    <t>Frog Is a Decomposer</t>
+  </si>
+  <si>
+    <t>Photosynthesis = Respiration</t>
+  </si>
+  <si>
+    <t>Photosynthesis &lt; Respiration</t>
+  </si>
+  <si>
+    <t>Photosynthesis &gt; Respiration</t>
+  </si>
+  <si>
+    <t>Photosynthesis = 0</t>
+  </si>
+  <si>
+    <t>Hawk Is a Consumer and Carnivore</t>
+  </si>
+  <si>
+    <t>Hawk Is a Consumer and Herbivore</t>
+  </si>
+  <si>
+    <t>Hawk Is a Decomposer</t>
+  </si>
+  <si>
+    <t>APAR X LUE</t>
+  </si>
+  <si>
+    <t>APAR + LUE</t>
+  </si>
+  <si>
+    <t>APAR - LUE</t>
+  </si>
+  <si>
+    <t>APAR / LUE</t>
+  </si>
+  <si>
+    <t>Tree --&gt; Frugivorous Birds --&gt; Hawk represents __________.</t>
+  </si>
+  <si>
+    <t>If we all became vegetarians, we'll be able to support our large populations. This can be explained through __________.</t>
+  </si>
+  <si>
+    <t>Consider the food chain: Grass --&gt; Grasshopper --&gt; Frog --&gt; Snake --&gt; Hawk. As we move up the food chain, __________.</t>
+  </si>
+  <si>
+    <t>available energy decreases</t>
+  </si>
+  <si>
+    <t>available energy increases</t>
+  </si>
+  <si>
+    <t>available energy remains the same</t>
+  </si>
+  <si>
+    <t>available energy Is zero everywhere</t>
+  </si>
+  <si>
+    <t>Glacial lakes are typical examples of __________.</t>
+  </si>
+  <si>
+    <t>Trees --&gt; Birds --&gt; Parasites --&gt; Hyperparasites represents __________.</t>
+  </si>
+  <si>
+    <t>Consider the food chain: Grass --&gt; Grasshopper --&gt; Frog --&gt; Snake --&gt; Hawk. In the food chain, __________.</t>
+  </si>
+  <si>
+    <t>Frog is a Producer</t>
+  </si>
+  <si>
+    <t>At the compensation point, __________.</t>
+  </si>
+  <si>
+    <t>Consider the food chain: Grass --&gt; Grasshopper --&gt; Frog --&gt; Snake --&gt; Hawk. In this food chain, __________.</t>
+  </si>
+  <si>
+    <t>more number of Hawks than Grasshopper can be supported</t>
+  </si>
+  <si>
+    <t>more number of Grasshoppers than Hawks can be supported</t>
+  </si>
+  <si>
+    <t>an equal number of Hawks and Grasshopper can be supported</t>
+  </si>
+  <si>
+    <t>Hawk is a Producer</t>
+  </si>
+  <si>
+    <t>Net Primary Productivity is given by __________.</t>
+  </si>
+  <si>
+    <t>Which of these is not a measure of absolute population density?</t>
+  </si>
+  <si>
+    <t>Total Count</t>
+  </si>
+  <si>
+    <t>Pelt Count</t>
+  </si>
+  <si>
+    <t>Capture-Recapture Method</t>
+  </si>
+  <si>
+    <t>Removal Method</t>
+  </si>
+  <si>
+    <t>100 Births</t>
+  </si>
+  <si>
+    <t>1000 Births</t>
+  </si>
+  <si>
+    <t>100 Live Births</t>
+  </si>
+  <si>
+    <t>1000 Live Births</t>
+  </si>
+  <si>
+    <t>_____ is how close the measured values are to the correct values</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Bias</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Simple Random Sampling</t>
+  </si>
+  <si>
+    <t>Systematic Sampling</t>
+  </si>
+  <si>
+    <t>Stratified Sampling</t>
+  </si>
+  <si>
+    <t>Multistage Sampling</t>
+  </si>
+  <si>
+    <t>Herpetofauna</t>
+  </si>
+  <si>
+    <t>Fishes</t>
+  </si>
+  <si>
+    <t>Large Mammals</t>
+  </si>
+  <si>
+    <t>Carnivores</t>
+  </si>
+  <si>
+    <t>I Shaped</t>
+  </si>
+  <si>
+    <t>J Shaped</t>
+  </si>
+  <si>
+    <t>S Shaped</t>
+  </si>
+  <si>
+    <t>O Shaped</t>
+  </si>
+  <si>
+    <t>Bees</t>
+  </si>
+  <si>
+    <t>Butterflies</t>
+  </si>
+  <si>
+    <t>Non-Pollinator Insects</t>
+  </si>
+  <si>
+    <t>Pollinator Insects</t>
+  </si>
+  <si>
+    <t>Which of these is true?</t>
+  </si>
+  <si>
+    <t>Physiological Longevity &gt; Ecological Longevity</t>
+  </si>
+  <si>
+    <t>Physiological Longevity = Ecological Longevity</t>
+  </si>
+  <si>
+    <t>Physiological Longevity &lt; Ecological Longevity</t>
+  </si>
+  <si>
+    <t>Physiological Longevity &gt;= Ecological Longevity</t>
+  </si>
+  <si>
+    <t>A sampling procedure such that each possible combination of sampling units out of the population has the same chance of being selected is referred to as __________.</t>
+  </si>
+  <si>
+    <t>The juvenile mortality rate is the annual number of deaths of juveniles per __________.</t>
+  </si>
+  <si>
+    <t>__________ employs a simple rule of selecting every kth unit starting with a number chosen at random from 1 to k as the random start.</t>
+  </si>
+  <si>
+    <t>Cover board surveys are typically used for sampling __________.</t>
+  </si>
+  <si>
+    <t>The minimum replacement level fertility for a population to grow should be greater than __________.</t>
+  </si>
+  <si>
+    <t>The logistic growth curve, when plotted, appears __________.</t>
+  </si>
+  <si>
+    <t>Pan traps are used for sampling __________.</t>
+  </si>
+  <si>
+    <t>0 to 10</t>
+  </si>
+  <si>
+    <t>0 to 50</t>
+  </si>
+  <si>
+    <t>0 to 100</t>
+  </si>
+  <si>
+    <t>0 to 300</t>
+  </si>
+  <si>
+    <t>Accidental Species</t>
+  </si>
+  <si>
+    <t>Indifferent Species</t>
+  </si>
+  <si>
+    <t>Selective Species</t>
+  </si>
+  <si>
+    <t>Exclusive Species</t>
+  </si>
+  <si>
+    <t>Which of these depicts correctly the lithosere primary succession?</t>
+  </si>
+  <si>
+    <t>Rock --&gt; Crustose Lichen --&gt; Foliose Lichen --&gt; Moss --&gt; Herbaceous Stage --&gt; Shrub --&gt; Woodland --&gt; Climax</t>
+  </si>
+  <si>
+    <t>Rock --&gt; Foliose Lichen --&gt; Crustose Lichen --&gt; Moss --&gt; Herbaceous Stage --&gt; Shrub --&gt; Woodland --&gt; Climax</t>
+  </si>
+  <si>
+    <t>Moss --&gt; Crustose Lichen --&gt; Foliose Lichen --&gt; Rock --&gt; Herbaceous Stage --&gt; Shrub --&gt; Woodland --&gt; Climax</t>
+  </si>
+  <si>
+    <t>Rock --&gt; Crustose Lichen --&gt; Foliose Lichen --&gt; Shrub --&gt; Herbaceous Stage --&gt; Moss --&gt; Woodland --&gt; Climax</t>
+  </si>
+  <si>
+    <t>Relative Density + Relative Frequency X Relative Dominance</t>
+  </si>
+  <si>
+    <t>Relative Density X Relative Frequency + Relative Dominance</t>
+  </si>
+  <si>
+    <t>Relative Density + Relative Frequency + Relative Dominance</t>
+  </si>
+  <si>
+    <t>Relative Density X Relative Frequency X Relative Dominance</t>
+  </si>
+  <si>
+    <t>Hydrosere</t>
+  </si>
+  <si>
+    <t>Xerosere</t>
+  </si>
+  <si>
+    <t>Psammosere</t>
+  </si>
+  <si>
+    <t>Halosere</t>
+  </si>
+  <si>
+    <t>Climatic Climax</t>
+  </si>
+  <si>
+    <t>Edaphic Climax</t>
+  </si>
+  <si>
+    <t>Disclimax</t>
+  </si>
+  <si>
+    <t>Catastrophic Climax</t>
+  </si>
+  <si>
+    <t>Which of these is correct?</t>
+  </si>
+  <si>
+    <t>Fundamental Niche &gt; Realized Niche</t>
+  </si>
+  <si>
+    <t>Fundamental Niche = Realized Niche</t>
+  </si>
+  <si>
+    <t>Fundamental Niche &lt; Realized Niche</t>
+  </si>
+  <si>
+    <t>Narrower Niche</t>
+  </si>
+  <si>
+    <t>Broader Niche</t>
+  </si>
+  <si>
+    <t>Same Size Niche</t>
+  </si>
+  <si>
+    <t>None of These</t>
+  </si>
+  <si>
+    <t>Ability to Grow on Bare Rocks</t>
+  </si>
+  <si>
+    <t>Ability to Tolerate Extreme Temperatures</t>
+  </si>
+  <si>
+    <t>Large Size</t>
+  </si>
+  <si>
+    <t>Short Lifespan</t>
+  </si>
+  <si>
+    <t>Fundamental Niche &gt;= Realized Niche</t>
+  </si>
+  <si>
+    <t>Which of these is not a characteristic of pioneer species?</t>
+  </si>
+  <si>
+    <t>When compared to generalist species, specialist species have __________.</t>
+  </si>
+  <si>
+    <t>A climax caused by wildfires is an example of __________.</t>
+  </si>
+  <si>
+    <t>The climax near Tindi village is being controlled by disturbance by cattle. This is an example of __________.</t>
+  </si>
+  <si>
+    <t>Lithosere is an example of __________.</t>
+  </si>
+  <si>
+    <t>Importance value can be written as __________.</t>
+  </si>
+  <si>
+    <t>A species found most frequently in a particular community, but also present occasionally in others is called __________.</t>
+  </si>
+  <si>
+    <t>Importance value varies from __________.</t>
+  </si>
+  <si>
+    <t>Chemical Factor</t>
+  </si>
+  <si>
+    <t>Demographic Factor</t>
+  </si>
+  <si>
+    <t>Push Factor</t>
+  </si>
+  <si>
+    <t>Pull Factor</t>
+  </si>
+  <si>
+    <t>Translocation</t>
+  </si>
+  <si>
+    <t>Migration</t>
+  </si>
+  <si>
+    <t>Dispersal</t>
+  </si>
+  <si>
+    <t>Drifting</t>
+  </si>
+  <si>
+    <t>Liebig’s Law of the Minimum</t>
+  </si>
+  <si>
+    <t>Liebig’s Law of the Maximum</t>
+  </si>
+  <si>
+    <t>Shelford’s Law of Tolerance</t>
+  </si>
+  <si>
+    <t>Shelford’s Law of Intolerance</t>
+  </si>
+  <si>
+    <t>Diffusion</t>
+  </si>
+  <si>
+    <t>Secular Dispersal</t>
+  </si>
+  <si>
+    <t>Jump Dispersal</t>
+  </si>
+  <si>
+    <t>Which of these is not a physical factor of habitat?</t>
+  </si>
+  <si>
+    <t>Soil</t>
+  </si>
+  <si>
+    <t>Moisture</t>
+  </si>
+  <si>
+    <t>Predators</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Potential Range</t>
+  </si>
+  <si>
+    <t>Effective Range</t>
+  </si>
+  <si>
+    <t>Actual Range</t>
+  </si>
+  <si>
+    <t>Economic Range</t>
+  </si>
+  <si>
+    <t>Autophagy</t>
+  </si>
+  <si>
+    <t>Allelophagy</t>
+  </si>
+  <si>
+    <t>Autopathy</t>
+  </si>
+  <si>
+    <t>Scarcity of food is a __________.</t>
+  </si>
+  <si>
+    <t>Good climate is a __________.</t>
+  </si>
+  <si>
+    <t>The movement of individuals away from their place of birth or hatching or seed production into a new habitat or area to survive and reproduce is called __________.</t>
+  </si>
+  <si>
+    <t>"The geographical distribution of a species will be controlled by that environmental factor for which the organism has the narrowest range of tolerance." This is the statement for __________.</t>
+  </si>
+  <si>
+    <t>"Quick movement over large distances, often across unsuitable terrain" is a description of __________.</t>
+  </si>
+  <si>
+    <t>The regular, seasonal movement of animals, often along fixed routes is called __________.</t>
+  </si>
+  <si>
+    <t>The movement of lions across the Gir landscape is an example of __________.</t>
+  </si>
+  <si>
+    <t>Transplantation experiments are used to find __________.</t>
+  </si>
+  <si>
+    <t>I tried growing vegetables under my teak plantation, but the vegetable plants died out. I should be concerned about __________.</t>
+  </si>
+  <si>
+    <t>In-situ conservation</t>
+  </si>
+  <si>
+    <t>Ex-situ conservation</t>
+  </si>
+  <si>
+    <t>In-situ preservation</t>
+  </si>
+  <si>
+    <t>Ex-situ preservation</t>
+  </si>
+  <si>
+    <t>Habitat</t>
+  </si>
+  <si>
+    <t>Ecosystem</t>
+  </si>
+  <si>
+    <t>Biome</t>
+  </si>
+  <si>
+    <t>Biosphere</t>
+  </si>
+  <si>
+    <t>Very High</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Very Low</t>
+  </si>
+  <si>
+    <t>Non-Existent</t>
+  </si>
+  <si>
+    <t>Environmental Variation</t>
+  </si>
+  <si>
+    <t>Forest Fire</t>
+  </si>
+  <si>
+    <t>Death Rate</t>
+  </si>
+  <si>
+    <t>Diseases</t>
+  </si>
+  <si>
+    <t>Habitat Loss</t>
+  </si>
+  <si>
+    <t>Habitat Enhancement</t>
+  </si>
+  <si>
+    <t>Invasive Species</t>
+  </si>
+  <si>
+    <t>Human Over Population</t>
+  </si>
+  <si>
+    <t>Original Forest --&gt; Dissection --&gt; Perforation --&gt; Fragmentation --&gt; Attrition</t>
+  </si>
+  <si>
+    <t>Original Forest --&gt; Dissection --&gt; Attrition --&gt; Fragmentation --&gt; Perforation</t>
+  </si>
+  <si>
+    <t>Original Forest --&gt; Dissection --&gt; Perforation --&gt; Attrition --&gt; Fragmentation</t>
+  </si>
+  <si>
+    <t>Original Forest --&gt; Dissection --&gt; Fragmentation --&gt; Perforation --&gt; Attrition</t>
+  </si>
+  <si>
+    <t>Pollination</t>
+  </si>
+  <si>
+    <t>Pollution</t>
+  </si>
+  <si>
+    <t>Birth Rate</t>
+  </si>
+  <si>
+    <t>Population Structures</t>
+  </si>
+  <si>
+    <t>Environmental Fluctuations</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>Gun</t>
+  </si>
+  <si>
+    <t>Cattle</t>
+  </si>
+  <si>
+    <t>Sickle</t>
+  </si>
+  <si>
+    <t>Captive breeding is an example of __________.</t>
+  </si>
+  <si>
+    <t>The "subset of physical and biotic environmental factors that permit an animal (or plant) to survive and reproduce" is the definition of __________.</t>
+  </si>
+  <si>
+    <t>We prefer those areas for the creation of a conservation reserve where the level of threat is __________.</t>
+  </si>
+  <si>
+    <t>Which of these is a deterministic factor?</t>
+  </si>
+  <si>
+    <t>The acronym HIPPO does not include __________.</t>
+  </si>
+  <si>
+    <t>Which of these correctly represents the process of habitat fragmentation and loss?</t>
+  </si>
+  <si>
+    <t>Which of these is a stochastic factor?</t>
+  </si>
+  <si>
+    <t>According to Leopold, which of these is not a tool of habitat management?</t>
+  </si>
+  <si>
+    <t>Zoo is an example of __________.</t>
+  </si>
+  <si>
+    <t>Which of these is a preventive check according to Malthus?</t>
+  </si>
+  <si>
+    <t>Foresight</t>
+  </si>
+  <si>
+    <t>Vice</t>
+  </si>
+  <si>
+    <t>Misery</t>
+  </si>
+  <si>
+    <t>Flood</t>
+  </si>
+  <si>
+    <t>Environmental Sustainability</t>
+  </si>
+  <si>
+    <t>Economic Sustainability</t>
+  </si>
+  <si>
+    <t>Trans-Boundary Sustainability</t>
+  </si>
+  <si>
+    <t>Social Sustainability</t>
+  </si>
+  <si>
+    <t>Screening</t>
+  </si>
+  <si>
+    <t>Scoping</t>
+  </si>
+  <si>
+    <t>Reporting</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>Which of these is a positive check according to Malthus?</t>
+  </si>
+  <si>
+    <t>Late Marriage</t>
+  </si>
+  <si>
+    <t>War</t>
+  </si>
+  <si>
+    <t>Celibacy</t>
+  </si>
+  <si>
+    <t>Moral Restraint</t>
+  </si>
+  <si>
+    <t>Industrial Sustainability</t>
+  </si>
+  <si>
+    <t>Agricultural Sustainability</t>
+  </si>
+  <si>
+    <t>High Birth Rate, High Death Rate to Low Birth Rate, Low Death Rate</t>
+  </si>
+  <si>
+    <t>Low Birth Rate, High Death Rate to Low Birth Rate, Low Death Rate</t>
+  </si>
+  <si>
+    <t>High Birth Rate, High Death Rate to Low Birth Rate, High Death Rate</t>
+  </si>
+  <si>
+    <t>Darwin</t>
+  </si>
+  <si>
+    <t>Spencer</t>
+  </si>
+  <si>
+    <t>Owens</t>
+  </si>
+  <si>
+    <t>I = P X A X T</t>
+  </si>
+  <si>
+    <t>I = P + A + T</t>
+  </si>
+  <si>
+    <t>I = P + A - T</t>
+  </si>
+  <si>
+    <t>I = P - (A + T)</t>
+  </si>
+  <si>
+    <t>Population grows in geometric progression, food supply increases in arithmetic progression</t>
+  </si>
+  <si>
+    <t>Population grows in geometric progression, food supply increases in geometric progression</t>
+  </si>
+  <si>
+    <t>Population grows in arithmetic progression, food supply increases in arithmetic progression</t>
+  </si>
+  <si>
+    <t>Population grows in arithmetic progression, food supply increases in geometric progression</t>
+  </si>
+  <si>
+    <t>Which of these is not a pillar of sustainability?</t>
+  </si>
+  <si>
+    <t>__________ is to identify which potential impacts are relevant to assess.</t>
+  </si>
+  <si>
+    <t>Which of these is a pillar of sustainability?</t>
+  </si>
+  <si>
+    <t>The demographic transition sees a society move from __________.</t>
+  </si>
+  <si>
+    <t>The book "An Essay on the Principle of Population" was written by __________.</t>
+  </si>
+  <si>
+    <t>The quantum of human impacts is given by __________.</t>
+  </si>
+  <si>
+    <t>__________ determines which projects or development require a full or partial impact assessment study.</t>
+  </si>
+  <si>
+    <t>According to Malthusian model __________.</t>
+  </si>
+  <si>
+    <t>Adaptation</t>
+  </si>
+  <si>
+    <t>Mitigation</t>
+  </si>
+  <si>
+    <t>Deceleration</t>
+  </si>
+  <si>
+    <t>Maladaptation</t>
+  </si>
+  <si>
+    <t>Which of these is not a climatic forcing for Earth?</t>
+  </si>
+  <si>
+    <t>Changes in plate tectonics</t>
+  </si>
+  <si>
+    <t>Changes in Earth's orbit</t>
+  </si>
+  <si>
+    <t>Changes in Moon's orbit</t>
+  </si>
+  <si>
+    <t>Changes in Sun's orbit</t>
+  </si>
+  <si>
+    <t>Ecological Integrity</t>
+  </si>
+  <si>
+    <t>Long-term Sustainability</t>
+  </si>
+  <si>
+    <t>Benefits and Engages Scientists</t>
+  </si>
+  <si>
+    <t>Informed by Past and Future</t>
+  </si>
+  <si>
+    <t>Adaptive Response</t>
+  </si>
+  <si>
+    <t>Adaptive Capacity</t>
+  </si>
+  <si>
+    <t>Mitigative Response</t>
+  </si>
+  <si>
+    <t>Mitigative Capacity</t>
+  </si>
+  <si>
+    <t>Short-term Sustainability</t>
+  </si>
+  <si>
+    <t>Benefits and Engages Society</t>
+  </si>
+  <si>
+    <t>Malmitigation</t>
+  </si>
+  <si>
+    <t>Changes in Sun's strength</t>
+  </si>
+  <si>
+    <t>Mesodebris in the context of plastic debris has fragments of size __________.</t>
+  </si>
+  <si>
+    <t>&gt; 20mm</t>
+  </si>
+  <si>
+    <t>5 - 20mm</t>
+  </si>
+  <si>
+    <t>&lt; 5mm</t>
+  </si>
+  <si>
+    <t>&lt; 1mm</t>
+  </si>
+  <si>
+    <t>The government came up with a regulation that incandescent bulbs be replaced by LED bulbs, so that electricity consumption and release of carbon dioxide from power plants is reduced. In the context change, such an action would be called __________.</t>
+  </si>
+  <si>
+    <t>Which of these is not a principle of ecological restoration?</t>
+  </si>
+  <si>
+    <t>"The ability of a system to adjust to climate change (including climate variability and extremes) to moderate potential damages, to take advantage of opportunities, or to cope with the consequences" is a definition for __________.</t>
+  </si>
+  <si>
+    <t>Macrodebris in context of plastic debris has fragments of size __________.</t>
+  </si>
+  <si>
+    <t>Because of climate change, Mudumalai Tiger Reserve is suffering from frequent droughts. The management has built several artificial water holes for animals, and fills them up regularly with tankers. In the context of climate change, such an action would be called __________.</t>
+  </si>
+  <si>
+    <t>"Any changes in natural and human systems that inadvertently increase vulnerability to climatic stimuli; an adaptation that does not succeed in reducing vulnerability but increases it instead" is a definition for __________.</t>
+  </si>
+  <si>
+    <t>It is increasing</t>
+  </si>
+  <si>
+    <t>It is not decreasing</t>
+  </si>
+  <si>
+    <t>It is causing some economic damage</t>
+  </si>
+  <si>
+    <t>It is causing excessive economic damage</t>
+  </si>
+  <si>
+    <t>Match Hypothesis</t>
+  </si>
+  <si>
+    <t>Mismatch Hypothesis</t>
+  </si>
+  <si>
+    <t>Match-Mismatch Hypothesis</t>
+  </si>
+  <si>
+    <t>R + G = M + F</t>
+  </si>
+  <si>
+    <t>R + M = G + F</t>
+  </si>
+  <si>
+    <t>R + F + M + G</t>
+  </si>
+  <si>
+    <t>R + G + M + F = 0</t>
+  </si>
+  <si>
+    <t>Decreasing harvesting rate</t>
+  </si>
+  <si>
+    <t>Constant harvesting rate</t>
+  </si>
+  <si>
+    <t>Increasing harvesting rate</t>
+  </si>
+  <si>
+    <t>Fluctuating harvesting rate</t>
+  </si>
+  <si>
+    <t>Phytoremediation</t>
+  </si>
+  <si>
+    <t>Biological Control</t>
+  </si>
+  <si>
+    <t>Biomagnification</t>
+  </si>
+  <si>
+    <t>Bioaccumulation</t>
+  </si>
+  <si>
+    <t>It is decreasing</t>
+  </si>
+  <si>
+    <t>It is not causing any economic damage</t>
+  </si>
+  <si>
+    <t>It is not causing excessive economic damage</t>
+  </si>
+  <si>
+    <t>Recovery</t>
+  </si>
+  <si>
+    <t>Restoration</t>
+  </si>
+  <si>
+    <t>Enhancement</t>
+  </si>
+  <si>
+    <t>Replacement</t>
+  </si>
+  <si>
+    <t>Lethal Effects</t>
+  </si>
+  <si>
+    <t>Sublethal Effects</t>
+  </si>
+  <si>
+    <t>Reduction of Existing Stressors</t>
+  </si>
+  <si>
+    <t>Reduce Fecundity</t>
+  </si>
+  <si>
+    <t>The maximum sustainable yield is near the beginning of the sigmoid curve</t>
+  </si>
+  <si>
+    <t>The maximum sustainable yield is near the mid point of the sigmoid curve</t>
+  </si>
+  <si>
+    <t>The maximum sustainable yield is near the end of the sigmoid curve</t>
+  </si>
+  <si>
+    <t>A pest population is called uncontrolled when __________.</t>
+  </si>
+  <si>
+    <t>The impact of El Niño on fishery collapse in Peru is explained by __________.</t>
+  </si>
+  <si>
+    <t>Ludwig's ratchet predicts __________.</t>
+  </si>
+  <si>
+    <t>A root zone treatment plant is an example of __________.</t>
+  </si>
+  <si>
+    <t>A pest population is called controlled when __________.</t>
+  </si>
+  <si>
+    <t>A deciduous forest in Madhya Pradesh was converted into a mine. After the mining operations were over, the pits were filled up with water and a lake was created. It is now visited by several migratory birds. This is an example of __________.</t>
+  </si>
+  <si>
+    <t>A deciduous forest in Madhya Pradesh was converted into a mine. After the mining operations were over, the pits were filled up with soil and species of deciduous forest planted again. This is an example of __________.</t>
+  </si>
+  <si>
+    <t>Which of these is not an impact of toxic chemicals?</t>
   </si>
 </sst>
 </file>
@@ -596,10 +1691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,6 +2099,1806 @@
         <v>79</v>
       </c>
     </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" t="s">
+        <v>97</v>
+      </c>
+      <c r="F26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" t="s">
+        <v>101</v>
+      </c>
+      <c r="F28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29" t="s">
+        <v>115</v>
+      </c>
+      <c r="C29" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" t="s">
+        <v>118</v>
+      </c>
+      <c r="F29" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" t="s">
+        <v>104</v>
+      </c>
+      <c r="E30" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>146</v>
+      </c>
+      <c r="B31" t="s">
+        <v>120</v>
+      </c>
+      <c r="C31" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" t="s">
+        <v>122</v>
+      </c>
+      <c r="E31" t="s">
+        <v>123</v>
+      </c>
+      <c r="F31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>147</v>
+      </c>
+      <c r="B32" t="s">
+        <v>124</v>
+      </c>
+      <c r="C32" t="s">
+        <v>125</v>
+      </c>
+      <c r="D32" t="s">
+        <v>126</v>
+      </c>
+      <c r="E32" t="s">
+        <v>127</v>
+      </c>
+      <c r="F32" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>148</v>
+      </c>
+      <c r="B33" t="s">
+        <v>149</v>
+      </c>
+      <c r="C33" t="s">
+        <v>150</v>
+      </c>
+      <c r="D33" t="s">
+        <v>151</v>
+      </c>
+      <c r="E33" t="s">
+        <v>152</v>
+      </c>
+      <c r="F33" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>153</v>
+      </c>
+      <c r="B34" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" t="s">
+        <v>129</v>
+      </c>
+      <c r="D34" t="s">
+        <v>130</v>
+      </c>
+      <c r="E34" t="s">
+        <v>131</v>
+      </c>
+      <c r="F34" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>154</v>
+      </c>
+      <c r="B35" t="s">
+        <v>120</v>
+      </c>
+      <c r="C35" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" t="s">
+        <v>122</v>
+      </c>
+      <c r="E35" t="s">
+        <v>123</v>
+      </c>
+      <c r="F35" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>155</v>
+      </c>
+      <c r="B36" t="s">
+        <v>156</v>
+      </c>
+      <c r="C36" t="s">
+        <v>132</v>
+      </c>
+      <c r="D36" t="s">
+        <v>133</v>
+      </c>
+      <c r="E36" t="s">
+        <v>134</v>
+      </c>
+      <c r="F36" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>157</v>
+      </c>
+      <c r="B37" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" t="s">
+        <v>136</v>
+      </c>
+      <c r="D37" t="s">
+        <v>137</v>
+      </c>
+      <c r="E37" t="s">
+        <v>138</v>
+      </c>
+      <c r="F37" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>158</v>
+      </c>
+      <c r="B38" t="s">
+        <v>159</v>
+      </c>
+      <c r="C38" t="s">
+        <v>160</v>
+      </c>
+      <c r="D38" t="s">
+        <v>161</v>
+      </c>
+      <c r="E38" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>158</v>
+      </c>
+      <c r="B39" t="s">
+        <v>162</v>
+      </c>
+      <c r="C39" t="s">
+        <v>139</v>
+      </c>
+      <c r="D39" t="s">
+        <v>140</v>
+      </c>
+      <c r="E39" t="s">
+        <v>141</v>
+      </c>
+      <c r="F39" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>163</v>
+      </c>
+      <c r="B40" t="s">
+        <v>142</v>
+      </c>
+      <c r="C40" t="s">
+        <v>143</v>
+      </c>
+      <c r="D40" t="s">
+        <v>144</v>
+      </c>
+      <c r="E40" t="s">
+        <v>145</v>
+      </c>
+      <c r="F40" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>164</v>
+      </c>
+      <c r="B41" t="s">
+        <v>165</v>
+      </c>
+      <c r="C41" t="s">
+        <v>166</v>
+      </c>
+      <c r="D41" t="s">
+        <v>167</v>
+      </c>
+      <c r="E41" t="s">
+        <v>168</v>
+      </c>
+      <c r="F41" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>200</v>
+      </c>
+      <c r="B42" t="s">
+        <v>169</v>
+      </c>
+      <c r="C42" t="s">
+        <v>170</v>
+      </c>
+      <c r="D42" t="s">
+        <v>171</v>
+      </c>
+      <c r="E42" t="s">
+        <v>172</v>
+      </c>
+      <c r="F42" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>173</v>
+      </c>
+      <c r="B43" t="s">
+        <v>174</v>
+      </c>
+      <c r="C43" t="s">
+        <v>175</v>
+      </c>
+      <c r="D43" t="s">
+        <v>176</v>
+      </c>
+      <c r="E43" t="s">
+        <v>177</v>
+      </c>
+      <c r="F43" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>201</v>
+      </c>
+      <c r="B44" t="s">
+        <v>178</v>
+      </c>
+      <c r="C44" t="s">
+        <v>179</v>
+      </c>
+      <c r="D44" t="s">
+        <v>180</v>
+      </c>
+      <c r="E44" t="s">
+        <v>181</v>
+      </c>
+      <c r="F44" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>202</v>
+      </c>
+      <c r="B45" t="s">
+        <v>182</v>
+      </c>
+      <c r="C45" t="s">
+        <v>183</v>
+      </c>
+      <c r="D45" t="s">
+        <v>184</v>
+      </c>
+      <c r="E45" t="s">
+        <v>185</v>
+      </c>
+      <c r="F45" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>203</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>3</v>
+      </c>
+      <c r="E46">
+        <v>4</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>204</v>
+      </c>
+      <c r="B47" t="s">
+        <v>186</v>
+      </c>
+      <c r="C47" t="s">
+        <v>187</v>
+      </c>
+      <c r="D47" t="s">
+        <v>188</v>
+      </c>
+      <c r="E47" t="s">
+        <v>189</v>
+      </c>
+      <c r="F47" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>205</v>
+      </c>
+      <c r="B48" t="s">
+        <v>190</v>
+      </c>
+      <c r="C48" t="s">
+        <v>191</v>
+      </c>
+      <c r="D48" t="s">
+        <v>192</v>
+      </c>
+      <c r="E48" t="s">
+        <v>193</v>
+      </c>
+      <c r="F48" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>199</v>
+      </c>
+      <c r="B49" t="s">
+        <v>178</v>
+      </c>
+      <c r="C49" t="s">
+        <v>179</v>
+      </c>
+      <c r="D49" t="s">
+        <v>180</v>
+      </c>
+      <c r="E49" t="s">
+        <v>181</v>
+      </c>
+      <c r="F49" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>194</v>
+      </c>
+      <c r="B50" t="s">
+        <v>195</v>
+      </c>
+      <c r="C50" t="s">
+        <v>196</v>
+      </c>
+      <c r="D50" t="s">
+        <v>197</v>
+      </c>
+      <c r="E50" t="s">
+        <v>198</v>
+      </c>
+      <c r="F50" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>251</v>
+      </c>
+      <c r="B51" t="s">
+        <v>206</v>
+      </c>
+      <c r="C51" t="s">
+        <v>207</v>
+      </c>
+      <c r="D51" t="s">
+        <v>208</v>
+      </c>
+      <c r="E51" t="s">
+        <v>209</v>
+      </c>
+      <c r="F51" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>250</v>
+      </c>
+      <c r="B52" t="s">
+        <v>210</v>
+      </c>
+      <c r="C52" t="s">
+        <v>211</v>
+      </c>
+      <c r="D52" t="s">
+        <v>212</v>
+      </c>
+      <c r="E52" t="s">
+        <v>213</v>
+      </c>
+      <c r="F52" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>214</v>
+      </c>
+      <c r="B53" t="s">
+        <v>215</v>
+      </c>
+      <c r="C53" t="s">
+        <v>216</v>
+      </c>
+      <c r="D53" t="s">
+        <v>217</v>
+      </c>
+      <c r="E53" t="s">
+        <v>218</v>
+      </c>
+      <c r="F53" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>249</v>
+      </c>
+      <c r="B54" t="s">
+        <v>219</v>
+      </c>
+      <c r="C54" t="s">
+        <v>220</v>
+      </c>
+      <c r="D54" t="s">
+        <v>221</v>
+      </c>
+      <c r="E54" t="s">
+        <v>222</v>
+      </c>
+      <c r="F54" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>248</v>
+      </c>
+      <c r="B55" t="s">
+        <v>223</v>
+      </c>
+      <c r="C55" t="s">
+        <v>224</v>
+      </c>
+      <c r="D55" t="s">
+        <v>225</v>
+      </c>
+      <c r="E55" t="s">
+        <v>226</v>
+      </c>
+      <c r="F55" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>247</v>
+      </c>
+      <c r="B56" t="s">
+        <v>227</v>
+      </c>
+      <c r="C56" t="s">
+        <v>228</v>
+      </c>
+      <c r="D56" t="s">
+        <v>229</v>
+      </c>
+      <c r="E56" t="s">
+        <v>230</v>
+      </c>
+      <c r="F56" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>246</v>
+      </c>
+      <c r="B57" t="s">
+        <v>227</v>
+      </c>
+      <c r="C57" t="s">
+        <v>228</v>
+      </c>
+      <c r="D57" t="s">
+        <v>229</v>
+      </c>
+      <c r="E57" t="s">
+        <v>230</v>
+      </c>
+      <c r="F57" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>231</v>
+      </c>
+      <c r="B58" t="s">
+        <v>232</v>
+      </c>
+      <c r="C58" t="s">
+        <v>233</v>
+      </c>
+      <c r="D58" t="s">
+        <v>234</v>
+      </c>
+      <c r="E58" t="s">
+        <v>243</v>
+      </c>
+      <c r="F58" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>245</v>
+      </c>
+      <c r="B59" t="s">
+        <v>235</v>
+      </c>
+      <c r="C59" t="s">
+        <v>236</v>
+      </c>
+      <c r="D59" t="s">
+        <v>237</v>
+      </c>
+      <c r="E59" t="s">
+        <v>238</v>
+      </c>
+      <c r="F59" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>244</v>
+      </c>
+      <c r="B60" t="s">
+        <v>239</v>
+      </c>
+      <c r="C60" t="s">
+        <v>240</v>
+      </c>
+      <c r="D60" t="s">
+        <v>241</v>
+      </c>
+      <c r="E60" t="s">
+        <v>242</v>
+      </c>
+      <c r="F60" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>279</v>
+      </c>
+      <c r="B61" t="s">
+        <v>252</v>
+      </c>
+      <c r="C61" t="s">
+        <v>253</v>
+      </c>
+      <c r="D61" t="s">
+        <v>254</v>
+      </c>
+      <c r="E61" t="s">
+        <v>255</v>
+      </c>
+      <c r="F61" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>280</v>
+      </c>
+      <c r="B62" t="s">
+        <v>252</v>
+      </c>
+      <c r="C62" t="s">
+        <v>253</v>
+      </c>
+      <c r="D62" t="s">
+        <v>254</v>
+      </c>
+      <c r="E62" t="s">
+        <v>255</v>
+      </c>
+      <c r="F62" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>281</v>
+      </c>
+      <c r="B63" t="s">
+        <v>256</v>
+      </c>
+      <c r="C63" t="s">
+        <v>257</v>
+      </c>
+      <c r="D63" t="s">
+        <v>258</v>
+      </c>
+      <c r="E63" t="s">
+        <v>259</v>
+      </c>
+      <c r="F63" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>282</v>
+      </c>
+      <c r="B64" t="s">
+        <v>260</v>
+      </c>
+      <c r="C64" t="s">
+        <v>261</v>
+      </c>
+      <c r="D64" t="s">
+        <v>262</v>
+      </c>
+      <c r="E64" t="s">
+        <v>263</v>
+      </c>
+      <c r="F64" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>283</v>
+      </c>
+      <c r="B65" t="s">
+        <v>264</v>
+      </c>
+      <c r="C65" t="s">
+        <v>265</v>
+      </c>
+      <c r="D65" t="s">
+        <v>266</v>
+      </c>
+      <c r="E65" t="s">
+        <v>259</v>
+      </c>
+      <c r="F65" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>284</v>
+      </c>
+      <c r="B66" t="s">
+        <v>256</v>
+      </c>
+      <c r="C66" t="s">
+        <v>257</v>
+      </c>
+      <c r="D66" t="s">
+        <v>258</v>
+      </c>
+      <c r="E66" t="s">
+        <v>259</v>
+      </c>
+      <c r="F66" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>285</v>
+      </c>
+      <c r="B67" t="s">
+        <v>264</v>
+      </c>
+      <c r="C67" t="s">
+        <v>265</v>
+      </c>
+      <c r="D67" t="s">
+        <v>266</v>
+      </c>
+      <c r="E67" t="s">
+        <v>259</v>
+      </c>
+      <c r="F67" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>267</v>
+      </c>
+      <c r="B68" t="s">
+        <v>268</v>
+      </c>
+      <c r="C68" t="s">
+        <v>269</v>
+      </c>
+      <c r="D68" t="s">
+        <v>270</v>
+      </c>
+      <c r="E68" t="s">
+        <v>271</v>
+      </c>
+      <c r="F68" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>286</v>
+      </c>
+      <c r="B69" t="s">
+        <v>272</v>
+      </c>
+      <c r="C69" t="s">
+        <v>273</v>
+      </c>
+      <c r="D69" t="s">
+        <v>274</v>
+      </c>
+      <c r="E69" t="s">
+        <v>275</v>
+      </c>
+      <c r="F69" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>287</v>
+      </c>
+      <c r="B70" t="s">
+        <v>276</v>
+      </c>
+      <c r="C70" t="s">
+        <v>277</v>
+      </c>
+      <c r="D70" t="s">
+        <v>278</v>
+      </c>
+      <c r="E70" t="s">
+        <v>93</v>
+      </c>
+      <c r="F70" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>321</v>
+      </c>
+      <c r="B71" t="s">
+        <v>288</v>
+      </c>
+      <c r="C71" t="s">
+        <v>289</v>
+      </c>
+      <c r="D71" t="s">
+        <v>290</v>
+      </c>
+      <c r="E71" t="s">
+        <v>291</v>
+      </c>
+      <c r="F71" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>322</v>
+      </c>
+      <c r="B72" t="s">
+        <v>292</v>
+      </c>
+      <c r="C72" t="s">
+        <v>293</v>
+      </c>
+      <c r="D72" t="s">
+        <v>294</v>
+      </c>
+      <c r="E72" t="s">
+        <v>295</v>
+      </c>
+      <c r="F72" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>323</v>
+      </c>
+      <c r="B73" t="s">
+        <v>296</v>
+      </c>
+      <c r="C73" t="s">
+        <v>297</v>
+      </c>
+      <c r="D73" t="s">
+        <v>298</v>
+      </c>
+      <c r="E73" t="s">
+        <v>299</v>
+      </c>
+      <c r="F73" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>324</v>
+      </c>
+      <c r="B74" t="s">
+        <v>300</v>
+      </c>
+      <c r="C74" t="s">
+        <v>301</v>
+      </c>
+      <c r="D74" t="s">
+        <v>302</v>
+      </c>
+      <c r="E74" t="s">
+        <v>303</v>
+      </c>
+      <c r="F74" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>325</v>
+      </c>
+      <c r="B75" t="s">
+        <v>304</v>
+      </c>
+      <c r="C75" t="s">
+        <v>305</v>
+      </c>
+      <c r="D75" t="s">
+        <v>306</v>
+      </c>
+      <c r="E75" t="s">
+        <v>307</v>
+      </c>
+      <c r="F75" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>326</v>
+      </c>
+      <c r="B76" t="s">
+        <v>308</v>
+      </c>
+      <c r="C76" t="s">
+        <v>309</v>
+      </c>
+      <c r="D76" t="s">
+        <v>310</v>
+      </c>
+      <c r="E76" t="s">
+        <v>311</v>
+      </c>
+      <c r="F76" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>325</v>
+      </c>
+      <c r="B77" t="s">
+        <v>304</v>
+      </c>
+      <c r="C77" t="s">
+        <v>306</v>
+      </c>
+      <c r="D77" t="s">
+        <v>312</v>
+      </c>
+      <c r="E77" t="s">
+        <v>313</v>
+      </c>
+      <c r="F77" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>327</v>
+      </c>
+      <c r="B78" t="s">
+        <v>314</v>
+      </c>
+      <c r="C78" t="s">
+        <v>302</v>
+      </c>
+      <c r="D78" t="s">
+        <v>315</v>
+      </c>
+      <c r="E78" t="s">
+        <v>316</v>
+      </c>
+      <c r="F78" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>328</v>
+      </c>
+      <c r="B79" t="s">
+        <v>317</v>
+      </c>
+      <c r="C79" t="s">
+        <v>318</v>
+      </c>
+      <c r="D79" t="s">
+        <v>319</v>
+      </c>
+      <c r="E79" t="s">
+        <v>320</v>
+      </c>
+      <c r="F79" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>329</v>
+      </c>
+      <c r="B80" t="s">
+        <v>288</v>
+      </c>
+      <c r="C80" t="s">
+        <v>289</v>
+      </c>
+      <c r="D80" t="s">
+        <v>290</v>
+      </c>
+      <c r="E80" t="s">
+        <v>291</v>
+      </c>
+      <c r="F80" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>330</v>
+      </c>
+      <c r="B81" t="s">
+        <v>331</v>
+      </c>
+      <c r="C81" t="s">
+        <v>332</v>
+      </c>
+      <c r="D81" t="s">
+        <v>333</v>
+      </c>
+      <c r="E81" t="s">
+        <v>334</v>
+      </c>
+      <c r="F81" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>364</v>
+      </c>
+      <c r="B82" t="s">
+        <v>335</v>
+      </c>
+      <c r="C82" t="s">
+        <v>336</v>
+      </c>
+      <c r="D82" t="s">
+        <v>337</v>
+      </c>
+      <c r="E82" t="s">
+        <v>338</v>
+      </c>
+      <c r="F82" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>365</v>
+      </c>
+      <c r="B83" t="s">
+        <v>339</v>
+      </c>
+      <c r="C83" t="s">
+        <v>340</v>
+      </c>
+      <c r="D83" t="s">
+        <v>341</v>
+      </c>
+      <c r="E83" t="s">
+        <v>342</v>
+      </c>
+      <c r="F83" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>343</v>
+      </c>
+      <c r="B84" t="s">
+        <v>344</v>
+      </c>
+      <c r="C84" t="s">
+        <v>345</v>
+      </c>
+      <c r="D84" t="s">
+        <v>346</v>
+      </c>
+      <c r="E84" t="s">
+        <v>347</v>
+      </c>
+      <c r="F84" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>366</v>
+      </c>
+      <c r="B85" t="s">
+        <v>338</v>
+      </c>
+      <c r="C85" t="s">
+        <v>348</v>
+      </c>
+      <c r="D85" t="s">
+        <v>349</v>
+      </c>
+      <c r="E85" t="s">
+        <v>337</v>
+      </c>
+      <c r="F85" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>367</v>
+      </c>
+      <c r="B86" t="s">
+        <v>350</v>
+      </c>
+      <c r="C86" t="s">
+        <v>351</v>
+      </c>
+      <c r="D86" t="s">
+        <v>352</v>
+      </c>
+      <c r="E86" t="s">
+        <v>350</v>
+      </c>
+      <c r="F86" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>368</v>
+      </c>
+      <c r="B87" t="s">
+        <v>353</v>
+      </c>
+      <c r="C87" t="s">
+        <v>13</v>
+      </c>
+      <c r="D87" t="s">
+        <v>354</v>
+      </c>
+      <c r="E87" t="s">
+        <v>355</v>
+      </c>
+      <c r="F87" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>369</v>
+      </c>
+      <c r="B88" t="s">
+        <v>356</v>
+      </c>
+      <c r="C88" t="s">
+        <v>357</v>
+      </c>
+      <c r="D88" t="s">
+        <v>358</v>
+      </c>
+      <c r="E88" t="s">
+        <v>359</v>
+      </c>
+      <c r="F88" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>370</v>
+      </c>
+      <c r="B89" t="s">
+        <v>339</v>
+      </c>
+      <c r="C89" t="s">
+        <v>340</v>
+      </c>
+      <c r="D89" t="s">
+        <v>341</v>
+      </c>
+      <c r="E89" t="s">
+        <v>342</v>
+      </c>
+      <c r="F89" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>371</v>
+      </c>
+      <c r="B90" t="s">
+        <v>360</v>
+      </c>
+      <c r="C90" t="s">
+        <v>361</v>
+      </c>
+      <c r="D90" t="s">
+        <v>362</v>
+      </c>
+      <c r="E90" t="s">
+        <v>363</v>
+      </c>
+      <c r="F90" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>393</v>
+      </c>
+      <c r="B91" t="s">
+        <v>394</v>
+      </c>
+      <c r="C91" t="s">
+        <v>395</v>
+      </c>
+      <c r="D91" t="s">
+        <v>396</v>
+      </c>
+      <c r="E91" t="s">
+        <v>397</v>
+      </c>
+      <c r="F91" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>398</v>
+      </c>
+      <c r="B92" t="s">
+        <v>372</v>
+      </c>
+      <c r="C92" t="s">
+        <v>373</v>
+      </c>
+      <c r="D92" t="s">
+        <v>374</v>
+      </c>
+      <c r="E92" t="s">
+        <v>375</v>
+      </c>
+      <c r="F92" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>376</v>
+      </c>
+      <c r="B93" t="s">
+        <v>377</v>
+      </c>
+      <c r="C93" t="s">
+        <v>378</v>
+      </c>
+      <c r="D93" t="s">
+        <v>379</v>
+      </c>
+      <c r="E93" t="s">
+        <v>380</v>
+      </c>
+      <c r="F93" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>399</v>
+      </c>
+      <c r="B94" t="s">
+        <v>381</v>
+      </c>
+      <c r="C94" t="s">
+        <v>382</v>
+      </c>
+      <c r="D94" t="s">
+        <v>383</v>
+      </c>
+      <c r="E94" t="s">
+        <v>384</v>
+      </c>
+      <c r="F94" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>400</v>
+      </c>
+      <c r="B95" t="s">
+        <v>385</v>
+      </c>
+      <c r="C95" t="s">
+        <v>386</v>
+      </c>
+      <c r="D95" t="s">
+        <v>387</v>
+      </c>
+      <c r="E95" t="s">
+        <v>388</v>
+      </c>
+      <c r="F95" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>399</v>
+      </c>
+      <c r="B96" t="s">
+        <v>381</v>
+      </c>
+      <c r="C96" t="s">
+        <v>389</v>
+      </c>
+      <c r="D96" t="s">
+        <v>390</v>
+      </c>
+      <c r="E96" t="s">
+        <v>384</v>
+      </c>
+      <c r="F96" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>401</v>
+      </c>
+      <c r="B97" t="s">
+        <v>394</v>
+      </c>
+      <c r="C97" t="s">
+        <v>395</v>
+      </c>
+      <c r="D97" t="s">
+        <v>396</v>
+      </c>
+      <c r="E97" t="s">
+        <v>397</v>
+      </c>
+      <c r="F97" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>402</v>
+      </c>
+      <c r="B98" t="s">
+        <v>372</v>
+      </c>
+      <c r="C98" t="s">
+        <v>373</v>
+      </c>
+      <c r="D98" t="s">
+        <v>374</v>
+      </c>
+      <c r="E98" t="s">
+        <v>375</v>
+      </c>
+      <c r="F98" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>403</v>
+      </c>
+      <c r="B99" t="s">
+        <v>372</v>
+      </c>
+      <c r="C99" t="s">
+        <v>373</v>
+      </c>
+      <c r="D99" t="s">
+        <v>375</v>
+      </c>
+      <c r="E99" t="s">
+        <v>391</v>
+      </c>
+      <c r="F99" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>376</v>
+      </c>
+      <c r="B100" t="s">
+        <v>377</v>
+      </c>
+      <c r="C100" t="s">
+        <v>378</v>
+      </c>
+      <c r="D100" t="s">
+        <v>380</v>
+      </c>
+      <c r="E100" t="s">
+        <v>392</v>
+      </c>
+      <c r="F100" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>437</v>
+      </c>
+      <c r="B101" t="s">
+        <v>404</v>
+      </c>
+      <c r="C101" t="s">
+        <v>405</v>
+      </c>
+      <c r="D101" t="s">
+        <v>406</v>
+      </c>
+      <c r="E101" t="s">
+        <v>407</v>
+      </c>
+      <c r="F101" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>438</v>
+      </c>
+      <c r="B102" t="s">
+        <v>408</v>
+      </c>
+      <c r="C102" t="s">
+        <v>409</v>
+      </c>
+      <c r="D102" t="s">
+        <v>410</v>
+      </c>
+      <c r="E102" t="s">
+        <v>40</v>
+      </c>
+      <c r="F102" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>231</v>
+      </c>
+      <c r="B103" t="s">
+        <v>411</v>
+      </c>
+      <c r="C103" t="s">
+        <v>412</v>
+      </c>
+      <c r="D103" t="s">
+        <v>413</v>
+      </c>
+      <c r="E103" t="s">
+        <v>414</v>
+      </c>
+      <c r="F103" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>439</v>
+      </c>
+      <c r="B104" t="s">
+        <v>415</v>
+      </c>
+      <c r="C104" t="s">
+        <v>416</v>
+      </c>
+      <c r="D104" t="s">
+        <v>417</v>
+      </c>
+      <c r="E104" t="s">
+        <v>418</v>
+      </c>
+      <c r="F104" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>440</v>
+      </c>
+      <c r="B105" t="s">
+        <v>419</v>
+      </c>
+      <c r="C105" t="s">
+        <v>420</v>
+      </c>
+      <c r="D105" t="s">
+        <v>421</v>
+      </c>
+      <c r="E105" t="s">
+        <v>422</v>
+      </c>
+      <c r="F105" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>441</v>
+      </c>
+      <c r="B106" t="s">
+        <v>404</v>
+      </c>
+      <c r="C106" t="s">
+        <v>423</v>
+      </c>
+      <c r="D106" t="s">
+        <v>424</v>
+      </c>
+      <c r="E106" t="s">
+        <v>425</v>
+      </c>
+      <c r="F106" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>442</v>
+      </c>
+      <c r="B107" t="s">
+        <v>426</v>
+      </c>
+      <c r="C107" t="s">
+        <v>427</v>
+      </c>
+      <c r="D107" t="s">
+        <v>428</v>
+      </c>
+      <c r="E107" t="s">
+        <v>429</v>
+      </c>
+      <c r="F107" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>443</v>
+      </c>
+      <c r="B108" t="s">
+        <v>426</v>
+      </c>
+      <c r="C108" t="s">
+        <v>427</v>
+      </c>
+      <c r="D108" t="s">
+        <v>428</v>
+      </c>
+      <c r="E108" t="s">
+        <v>429</v>
+      </c>
+      <c r="F108" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>444</v>
+      </c>
+      <c r="B109" t="s">
+        <v>430</v>
+      </c>
+      <c r="C109" t="s">
+        <v>431</v>
+      </c>
+      <c r="D109" t="s">
+        <v>432</v>
+      </c>
+      <c r="E109" t="s">
+        <v>433</v>
+      </c>
+      <c r="F109" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>231</v>
+      </c>
+      <c r="B110" t="s">
+        <v>434</v>
+      </c>
+      <c r="C110" t="s">
+        <v>435</v>
+      </c>
+      <c r="D110" t="s">
+        <v>436</v>
+      </c>
+      <c r="E110" t="s">
+        <v>40</v>
+      </c>
+      <c r="F110" t="s">
+        <v>435</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>